<commit_message>
Tugas 1 (Implementasi Import pada Semua Tabel)
</commit_message>
<xml_diff>
--- a/Minggu8/PWL_POS/public/template_barang.xlsx
+++ b/Minggu8/PWL_POS/public/template_barang.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\PWL_2025\Minggu8\PWL_POS\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{837A2E43-B1F2-4247-BD53-7C79E19C69B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D8AB16E-F877-4861-8EB1-1F2E13A579D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{CEA3B3E8-2FAC-4672-9848-A4A814AAD48B}"/>
+    <workbookView xWindow="7200" yWindow="585" windowWidth="21600" windowHeight="11295" xr2:uid="{CEA3B3E8-2FAC-4672-9848-A4A814AAD48B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,9 +27,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
-    <t>kateori_id</t>
-  </si>
-  <si>
     <t>barang_kode</t>
   </si>
   <si>
@@ -70,6 +67,9 @@
   </si>
   <si>
     <t>Action Figure</t>
+  </si>
+  <si>
+    <t>kategori_id</t>
   </si>
 </sst>
 </file>
@@ -424,7 +424,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -438,19 +438,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -458,10 +458,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D2">
         <v>5000</v>
@@ -475,10 +475,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D3">
         <v>3500</v>
@@ -492,10 +492,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D4">
         <v>65000</v>
@@ -509,10 +509,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D5">
         <v>500</v>
@@ -526,10 +526,10 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D6">
         <v>150000</v>

</xml_diff>